<commit_message>
Subo todos los archivos del proyecto
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,6 +731,156 @@
         <v>7534</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>14.123.220-7</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>gggtg</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>14.123.220-7</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>afre</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Validación Microchip, Vacuna Antirábica, Vacuna Polivalente</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14.123.220-7</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Vacuna Antirábica</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>9186</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>14.123.220-7</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Colins</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>9186</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>14.123.220-7</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>asas</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Vacuna Triple Felina</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>9186</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>14.123.220-7</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>lesto</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>9186</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualiza estilo y agrega reinicio de base de datos
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Número Atención</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +489,7 @@
       <c r="E2" t="n">
         <v>4352</v>
       </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -505,6 +511,7 @@
       <c r="E3" t="n">
         <v>4352</v>
       </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -530,6 +537,7 @@
       <c r="E4" t="n">
         <v>4352</v>
       </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -555,6 +563,7 @@
       <c r="E5" t="n">
         <v>4352</v>
       </c>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -580,6 +589,7 @@
       <c r="E6" t="n">
         <v>4352</v>
       </c>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -605,6 +615,7 @@
       <c r="E7" t="n">
         <v>7276</v>
       </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -630,6 +641,7 @@
       <c r="E8" t="n">
         <v>7276</v>
       </c>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -655,6 +667,7 @@
       <c r="E9" t="n">
         <v>9362</v>
       </c>
+      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -680,6 +693,7 @@
       <c r="E10" t="n">
         <v>7252</v>
       </c>
+      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -705,6 +719,7 @@
       <c r="E11" t="n">
         <v>7252</v>
       </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -730,6 +745,7 @@
       <c r="E12" t="n">
         <v>7534</v>
       </c>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -755,6 +771,7 @@
       <c r="E13" t="n">
         <v>1167</v>
       </c>
+      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -780,6 +797,7 @@
       <c r="E14" t="n">
         <v>1167</v>
       </c>
+      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -805,6 +823,7 @@
       <c r="E15" t="n">
         <v>9186</v>
       </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -830,6 +849,7 @@
       <c r="E16" t="n">
         <v>9186</v>
       </c>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -855,6 +875,7 @@
       <c r="E17" t="n">
         <v>9186</v>
       </c>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -879,6 +900,179 @@
       </c>
       <c r="E18" t="n">
         <v>9186</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>23947208-7</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>liu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Validación Microchip, Vacuna Antirábica, Vacuna Triple Felina</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2249</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>23947208-7</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Miausss</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Vacuna Antirábica, Vacuna Polivalente</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>2249</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ratso</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>8155</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-05-09 14:39:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Dibu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2428</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-05-09 14:40:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>laz99</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Validación Microchip, Vacuna Polivalente</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>8794</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-09 15:00:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>al fin</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2602</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-09 15:22:11</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sube todos los cambios recientes al módulo de atención
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,67 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sfaz/modulo_atencion/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6514332F-2D1B-044F-9353-A03B78103EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Servicios</t>
-  </si>
-  <si>
-    <t>Número Atención</t>
-  </si>
-  <si>
-    <t>Fecha y Hora</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,42 +420,352 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>RUT</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Servicios</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Número Atención</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1356</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:20:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>4865</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:32:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>6927</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:34:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Validación Microchip, Aplicación Microchip</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>6927</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:34:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Validación Microchip, Aplicación Microchip, Vacuna Antirábica</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>6927</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:34:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Validación Microchip, Aplicación Microchip, Vacuna Antirábica, Vacuna Polivalente</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>6927</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:34:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Vacuna Polivalente, Vacuna Triple Felina</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>6927</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:34:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>yaya</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Vacuna Triple Felina</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>4046</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:37:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>hahah</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>6403</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:37:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3970598-2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>benja</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1333</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-05-09 21:38:57</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{3aebaaad-7943-488e-8a4c-7379a9fc7933}" enabled="1" method="Standard" siteId="{326c2335-66a0-4d53-aa59-0afa0692c5b2}" contentBits="0" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Corrige guardado de número de atención y lo exporta en el Excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -1,80 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sfaz/modulo_atencion/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A490B862-128E-AC45-9A72-C5F9E00016F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Servicios</t>
-  </si>
-  <si>
-    <t>Número Atención</t>
-  </si>
-  <si>
-    <t>Fecha y Hora</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,48 +420,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="A2:G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>RUT</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Servicios</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Número Atención</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>17083851-3</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>linda</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Aplicación Microchip</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>9084</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-06-06 11:36:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>17083851-3</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>isi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Aplicación Microchip</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-06 11:49:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>17083851-3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Yaz</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Vacuna Antirábica</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-06 11:56:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>17083851-3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>miauus</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gato</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Vacuna Polivalente</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-06 12:20:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>13839414-k</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rac</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Perro</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Validación Microchip</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-06 12:29:15</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{3aebaaad-7943-488e-8a4c-7379a9fc7933}" enabled="1" method="Standard" siteId="{326c2335-66a0-4d53-aa59-0afa0692c5b2}" contentBits="0" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>